<commit_message>
usable version of ChibiPoint with evaluation turned off
</commit_message>
<xml_diff>
--- a/evaluationStudy/analyses/PilotStudy.xlsx
+++ b/evaluationStudy/analyses/PilotStudy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="420" windowWidth="30540" windowHeight="20660" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="38400" windowHeight="21080" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -128,8 +128,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -178,7 +182,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -194,6 +198,8 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -209,6 +215,8 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -277,63 +285,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$1</c:f>
+              <c:f>Sheet1!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>ChibiPoint (crosshairs)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ChibiPoint (crosshairs AND flyouts)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -349,6 +305,58 @@
                   <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ChibiPoint (crosshairs AND flyouts)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
@@ -381,7 +389,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$A$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -393,7 +401,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$10</c:f>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -437,11 +445,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2114082264"/>
-        <c:axId val="2114925336"/>
+        <c:axId val="2063512856"/>
+        <c:axId val="2063534808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2114082264"/>
+        <c:axId val="2063512856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -474,15 +482,15 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2114925336"/>
+        <c:crossAx val="2063534808"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
+        <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2114925336"/>
+        <c:axId val="2063534808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -512,7 +520,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2114082264"/>
+        <c:crossAx val="2063512856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="2.0"/>
@@ -585,63 +593,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$1</c:f>
+              <c:f>Sheet1!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>ChibiPoint (crosshairs)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ChibiPoint (crosshairs AND flyouts)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -657,6 +613,58 @@
                   <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ChibiPoint (crosshairs AND flyouts)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
@@ -689,7 +697,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$A$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -701,7 +709,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$10</c:f>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -745,11 +753,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2122831848"/>
-        <c:axId val="2120570216"/>
+        <c:axId val="2113173960"/>
+        <c:axId val="2113179560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2122831848"/>
+        <c:axId val="2113173960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -782,7 +790,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2120570216"/>
+        <c:crossAx val="2113179560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -790,7 +798,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2120570216"/>
+        <c:axId val="2113179560"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -821,7 +829,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122831848"/>
+        <c:crossAx val="2113173960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1055,11 +1063,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2126017336"/>
-        <c:axId val="2115917032"/>
+        <c:axId val="-2116469800"/>
+        <c:axId val="-2116626200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2126017336"/>
+        <c:axId val="-2116469800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1087,7 +1095,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115917032"/>
+        <c:crossAx val="-2116626200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1095,7 +1103,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2115917032"/>
+        <c:axId val="-2116626200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1125,7 +1133,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126017336"/>
+        <c:crossAx val="-2116469800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1357,11 +1365,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2126788968"/>
-        <c:axId val="2122182904"/>
+        <c:axId val="2063521768"/>
+        <c:axId val="2063373928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2126788968"/>
+        <c:axId val="2063521768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1389,7 +1397,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122182904"/>
+        <c:crossAx val="2063373928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1397,7 +1405,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2122182904"/>
+        <c:axId val="2063373928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1427,7 +1435,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126788968"/>
+        <c:crossAx val="2063521768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1543,11 +1551,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2147097880"/>
-        <c:axId val="2125635272"/>
+        <c:axId val="2142867704"/>
+        <c:axId val="2128074488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2147097880"/>
+        <c:axId val="2142867704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1575,7 +1583,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125635272"/>
+        <c:crossAx val="2128074488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1583,7 +1591,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2125635272"/>
+        <c:axId val="2128074488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5.0"/>
@@ -1615,7 +1623,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2147097880"/>
+        <c:crossAx val="2142867704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="1.0"/>
@@ -1732,11 +1740,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2146714360"/>
-        <c:axId val="-2146893496"/>
+        <c:axId val="-2117428872"/>
+        <c:axId val="2129467816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2146714360"/>
+        <c:axId val="-2117428872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1764,7 +1772,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146893496"/>
+        <c:crossAx val="2129467816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1772,7 +1780,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2146893496"/>
+        <c:axId val="2129467816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5.0"/>
@@ -1799,7 +1807,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146714360"/>
+        <c:crossAx val="-2117428872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="1.0"/>
@@ -1911,11 +1919,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2118338504"/>
-        <c:axId val="2118697432"/>
+        <c:axId val="2128216824"/>
+        <c:axId val="2128634680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2118338504"/>
+        <c:axId val="2128216824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1943,7 +1951,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2118697432"/>
+        <c:crossAx val="2128634680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1951,7 +1959,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2118697432"/>
+        <c:axId val="2128634680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1982,7 +1990,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2118338504"/>
+        <c:crossAx val="2128216824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="1.0"/>
@@ -2559,8 +2567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2572,112 +2580,112 @@
   <sheetData>
     <row r="1" spans="1:3" ht="177">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>3</v>
       </c>
       <c r="C2">
-        <v>33</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
+        <v>48</v>
+      </c>
+      <c r="B3">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>8</v>
-      </c>
-      <c r="C3">
-        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>3</v>
-      </c>
-      <c r="C4">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
+        <v>44</v>
+      </c>
+      <c r="B5">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>4</v>
-      </c>
-      <c r="C5">
-        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>3</v>
-      </c>
-      <c r="C6">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
+        <v>222</v>
+      </c>
+      <c r="B7">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>2</v>
-      </c>
-      <c r="C7">
-        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>3</v>
       </c>
       <c r="C8">
-        <v>25</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
+        <v>23</v>
+      </c>
+      <c r="B9">
         <v>5</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>8</v>
-      </c>
-      <c r="C9">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
+        <v>49</v>
+      </c>
+      <c r="B10">
         <v>6</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>3</v>
-      </c>
-      <c r="C10">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -2963,8 +2971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3033,13 +3041,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="184">
+    <row r="1" spans="1:7" ht="177">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>

</xml_diff>